<commit_message>
proje etiketleri tamamlandı ve projelere başlandı
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ataba\Desktop\works\github\oonio-crm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8287FA4A-B23F-4E3C-9873-056C9CF06770}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D5639F-485F-4182-8352-A2F434D1C38F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>users</t>
   </si>
@@ -54,50 +54,140 @@
     <t>user_extra</t>
   </si>
   <si>
-    <t>customers</t>
-  </si>
-  <si>
-    <t>customer_id</t>
-  </si>
-  <si>
-    <t>customer_name</t>
-  </si>
-  <si>
-    <t>customer_email</t>
-  </si>
-  <si>
-    <t>customer_phone</t>
-  </si>
-  <si>
-    <t>customer_mobile</t>
-  </si>
-  <si>
-    <t>customer_address</t>
-  </si>
-  <si>
-    <t>customer_extra</t>
-  </si>
-  <si>
     <t>user_c_time</t>
   </si>
   <si>
     <t>user_u_time</t>
   </si>
   <si>
-    <t>customer_c_time</t>
-  </si>
-  <si>
-    <t>customer_u_time</t>
-  </si>
-  <si>
-    <t>customer_gender</t>
+    <t>contacts</t>
+  </si>
+  <si>
+    <t>contact_id</t>
+  </si>
+  <si>
+    <t>contact_name</t>
+  </si>
+  <si>
+    <t>contact_gender</t>
+  </si>
+  <si>
+    <t>contact_email</t>
+  </si>
+  <si>
+    <t>contact_mobile</t>
+  </si>
+  <si>
+    <t>contact_phone</t>
+  </si>
+  <si>
+    <t>contact_address</t>
+  </si>
+  <si>
+    <t>contact_extra</t>
+  </si>
+  <si>
+    <t>contact_c_time</t>
+  </si>
+  <si>
+    <t>contact_u_time</t>
+  </si>
+  <si>
+    <t>projects</t>
+  </si>
+  <si>
+    <t>project_id</t>
+  </si>
+  <si>
+    <t>taxonomies</t>
+  </si>
+  <si>
+    <t>tax_id</t>
+  </si>
+  <si>
+    <t>tax_key</t>
+  </si>
+  <si>
+    <t>tax_val</t>
+  </si>
+  <si>
+    <t>tax_parent</t>
+  </si>
+  <si>
+    <t>tax keys</t>
+  </si>
+  <si>
+    <t>project_taxonomy</t>
+  </si>
+  <si>
+    <t>project_contact</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>project_content</t>
+  </si>
+  <si>
+    <t>project_c_time</t>
+  </si>
+  <si>
+    <t>project_u_time</t>
+  </si>
+  <si>
+    <t>project_status</t>
+  </si>
+  <si>
+    <t>project_user</t>
+  </si>
+  <si>
+    <t>project_title</t>
+  </si>
+  <si>
+    <t>project_description</t>
+  </si>
+  <si>
+    <t>media_id</t>
+  </si>
+  <si>
+    <t>media_title</t>
+  </si>
+  <si>
+    <t>media_description</t>
+  </si>
+  <si>
+    <t>media_type</t>
+  </si>
+  <si>
+    <t>media_mime_type</t>
+  </si>
+  <si>
+    <t>media_path</t>
+  </si>
+  <si>
+    <t>media_c_time</t>
+  </si>
+  <si>
+    <t>project_media</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>project_extra</t>
+  </si>
+  <si>
+    <t>tax_extra</t>
+  </si>
+  <si>
+    <t>project_tag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,13 +195,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -126,8 +270,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,126 +560,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C48"/>
+  <dimension ref="B1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" activeCellId="9" sqref="C2 C3 C4 C5 C6 C7 C8 C9 C10 C11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bs5 switch radio for users
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ataba\Desktop\works\github\oonio-crm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7313C443-100C-4140-BDA5-C46039607F2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173B391D-F1D9-43F2-8EC4-258E71E104D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,7 +187,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,15 +208,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -278,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -288,7 +279,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,7 +562,7 @@
   <dimension ref="B1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" activeCellId="2" sqref="F1 F6 F11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,10 +587,10 @@
       <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>30</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -697,7 +687,7 @@
       <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>31</v>
       </c>
       <c r="G6" t="s">
@@ -773,7 +763,7 @@
       <c r="D11" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>